<commit_message>
Some further error corrections when working with the marks sheet
</commit_message>
<xml_diff>
--- a/Report Creator/test_subjects/Marks Sheet Term II 2024/A level Marks Sheet Term II 2024/Marksheet A level - ART.xlsx
+++ b/Report Creator/test_subjects/Marks Sheet Term II 2024/A level Marks Sheet Term II 2024/Marksheet A level - ART.xlsx
@@ -180,13 +180,16 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1737,10 +1740,18 @@
         <v>32</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="D7" s="3">
+        <v>75.0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>70.0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>86.0</v>
+      </c>
+      <c r="G7" s="3">
+        <v>66.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="B8" s="1" t="s">
@@ -1777,10 +1788,18 @@
         <v>36</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="D11" s="3">
+        <v>68.0</v>
+      </c>
+      <c r="E11" s="3">
+        <v>54.0</v>
+      </c>
+      <c r="F11" s="3">
+        <v>65.0</v>
+      </c>
+      <c r="G11" s="3">
+        <v>54.0</v>
+      </c>
     </row>
     <row r="12">
       <c r="B12" s="1" t="s">
@@ -1807,10 +1826,18 @@
         <v>39</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="D14" s="3">
+        <v>72.0</v>
+      </c>
+      <c r="E14" s="3">
+        <v>68.0</v>
+      </c>
+      <c r="F14" s="3">
+        <v>70.0</v>
+      </c>
+      <c r="G14" s="3">
+        <v>54.0</v>
+      </c>
     </row>
     <row r="15">
       <c r="B15" s="1" t="s">

</xml_diff>